<commit_message>
fix: ultima version del excel
</commit_message>
<xml_diff>
--- a/Tablas.xlsx
+++ b/Tablas.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="32">
   <si>
     <t>TIPO_ENVIO</t>
   </si>
@@ -101,6 +101,9 @@
     <t>PK</t>
   </si>
   <si>
+    <t>Medida/Atributo</t>
+  </si>
+  <si>
     <t>Media</t>
   </si>
   <si>
@@ -108,6 +111,9 @@
   </si>
   <si>
     <t>FAC_ORDENES</t>
+  </si>
+  <si>
+    <t>Media/Atributo</t>
   </si>
 </sst>
 </file>
@@ -677,11 +683,11 @@
     </row>
   </sheetData>
   <mergeCells count="5">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:M1"/>
     <mergeCell ref="N1:R1"/>
-    <mergeCell ref="I1:M1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="A1:D1"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -797,11 +803,11 @@
       <c r="A4" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>26</v>
+      <c r="B4" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>27</v>
       </c>
       <c r="D4" s="15" t="s">
         <v>26</v>
@@ -813,10 +819,10 @@
         <v>26</v>
       </c>
       <c r="G4" s="16" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H4" s="16" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I4" s="15" t="s">
         <v>26</v>
@@ -827,7 +833,7 @@
     </row>
     <row r="7">
       <c r="A7" s="17" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -843,10 +849,10 @@
       <c r="A8" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="16" t="s">
         <v>8</v>
       </c>
       <c r="D8" s="15" t="s">
@@ -875,11 +881,11 @@
       <c r="A9" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>26</v>
+      <c r="B9" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>31</v>
       </c>
       <c r="D9" s="15" t="s">
         <v>26</v>
@@ -891,10 +897,10 @@
         <v>26</v>
       </c>
       <c r="G9" s="16" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H9" s="16" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I9" s="15" t="s">
         <v>26</v>
@@ -934,7 +940,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3"/>
@@ -1005,10 +1011,10 @@
     </row>
   </sheetData>
   <mergeCells count="4">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:F1"/>
-    <mergeCell ref="C1:D1"/>
     <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A1:B1"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>